<commit_message>
edit column names in excel
</commit_message>
<xml_diff>
--- a/data/20181210_eag_info.xlsx
+++ b/data/20181210_eag_info.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\k\01projekt\17026004_WATERNET_Waterbalansen\05pyfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\k\01projekt\17026004_WATERNET_Waterbalansen\05pyfiles\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24E9114-0AE0-4133-895C-AF8CD77E346D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4194BD9D-5C5E-4B75-8577-A71643583C91}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7725" activeTab="1" xr2:uid="{D42CEE2B-2D61-4AA0-9082-ECF2208A28A8}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="292">
   <si>
     <t>ID</t>
   </si>
@@ -909,6 +909,21 @@
   </si>
   <si>
     <t>Hier staan ALLEEN de kolomnamen voor reeksen MET DATA uit de uitgangspunten sheet van de Excelfiles</t>
+  </si>
+  <si>
+    <t>Uitlaat1</t>
+  </si>
+  <si>
+    <t>Gemaal1</t>
+  </si>
+  <si>
+    <t>Gemaal2</t>
+  </si>
+  <si>
+    <t>Gemaal3</t>
+  </si>
+  <si>
+    <t>Gemaal4</t>
   </si>
 </sst>
 </file>
@@ -1194,25 +1209,25 @@
     <tableColumn id="2" xr3:uid="{FEA2244A-36C6-4F74-B58F-FB49D89DD0CC}" uniqueName="2" name="Neerslag" queryTableFieldId="2" dataDxfId="37"/>
     <tableColumn id="3" xr3:uid="{C49BF7A5-0F26-44EA-BC98-5CEF0772D30C}" uniqueName="3" name="Verdamping" queryTableFieldId="3" dataDxfId="36"/>
     <tableColumn id="4" xr3:uid="{A7163F6B-1176-4B2E-8307-A9A79372D676}" uniqueName="4" name="Peil" queryTableFieldId="4" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{67EE6766-4720-4FC8-ADA1-AC30BCB9E382}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{3452F98B-458D-422A-9EAC-3BA6259A959F}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{E2BBD6F6-1AFB-4AF2-A6DB-C1B78A7D8E7E}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="32"/>
-    <tableColumn id="8" xr3:uid="{D8E8BA9C-B2E0-4A39-A11D-F29FCC5B8608}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{67EE6766-4720-4FC8-ADA1-AC30BCB9E382}" uniqueName="5" name="Gemaal1" queryTableFieldId="5" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{3452F98B-458D-422A-9EAC-3BA6259A959F}" uniqueName="6" name="Gemaal2" queryTableFieldId="6" dataDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{E2BBD6F6-1AFB-4AF2-A6DB-C1B78A7D8E7E}" uniqueName="7" name="Gemaal3" queryTableFieldId="7" dataDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{D8E8BA9C-B2E0-4A39-A11D-F29FCC5B8608}" uniqueName="8" name="Gemaal4" queryTableFieldId="8" dataDxfId="31"/>
     <tableColumn id="9" xr3:uid="{72B32F7F-D21D-4B36-B0C0-2260DCB96323}" uniqueName="9" name="Inlaat voor calibratie" queryTableFieldId="9" dataDxfId="30"/>
     <tableColumn id="10" xr3:uid="{D02B5E2F-FB46-441A-A699-CCF8EBCFDD16}" uniqueName="10" name="gemengd gerioleerd stelsel m3/d/ha" queryTableFieldId="10" dataDxfId="29"/>
-    <tableColumn id="11" xr3:uid="{F04540CE-2CAF-4EBF-B51E-4CC6BD370C76}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="28"/>
-    <tableColumn id="12" xr3:uid="{A2C87C34-3238-4479-AC31-07AE603A509A}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="27"/>
-    <tableColumn id="13" xr3:uid="{816668FE-6184-4D7F-B44B-D2FC05326D93}" uniqueName="13" name="Column13" queryTableFieldId="13" dataDxfId="26"/>
-    <tableColumn id="14" xr3:uid="{EA0BC37D-0CEB-4296-82C3-501C31DBA056}" uniqueName="14" name="Column14" queryTableFieldId="14" dataDxfId="25"/>
-    <tableColumn id="15" xr3:uid="{B3CE4A0B-0D02-4C8C-A562-227658C3108E}" uniqueName="15" name="Column15" queryTableFieldId="15" dataDxfId="24"/>
-    <tableColumn id="16" xr3:uid="{E1CB06E9-17AD-4E15-9093-F178C4020DCB}" uniqueName="16" name="Column16" queryTableFieldId="16" dataDxfId="23"/>
-    <tableColumn id="17" xr3:uid="{EABA0519-4E9E-4B4C-A8E0-09ECE0028650}" uniqueName="17" name="Column17" queryTableFieldId="17" dataDxfId="22"/>
-    <tableColumn id="18" xr3:uid="{44A642CC-6F94-4E75-9796-1E854132BDCF}" uniqueName="18" name="Column18" queryTableFieldId="18" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{F04540CE-2CAF-4EBF-B51E-4CC6BD370C76}" uniqueName="11" name="Inlaat1" queryTableFieldId="11" dataDxfId="28"/>
+    <tableColumn id="12" xr3:uid="{A2C87C34-3238-4479-AC31-07AE603A509A}" uniqueName="12" name="Inlaat2" queryTableFieldId="12" dataDxfId="27"/>
+    <tableColumn id="13" xr3:uid="{816668FE-6184-4D7F-B44B-D2FC05326D93}" uniqueName="13" name="Inlaat3" queryTableFieldId="13" dataDxfId="26"/>
+    <tableColumn id="14" xr3:uid="{EA0BC37D-0CEB-4296-82C3-501C31DBA056}" uniqueName="14" name="Inlaat4" queryTableFieldId="14" dataDxfId="25"/>
+    <tableColumn id="15" xr3:uid="{B3CE4A0B-0D02-4C8C-A562-227658C3108E}" uniqueName="15" name="Uitlaat1" queryTableFieldId="15" dataDxfId="24"/>
+    <tableColumn id="16" xr3:uid="{E1CB06E9-17AD-4E15-9093-F178C4020DCB}" uniqueName="16" name="Uitlaat2" queryTableFieldId="16" dataDxfId="23"/>
+    <tableColumn id="17" xr3:uid="{EABA0519-4E9E-4B4C-A8E0-09ECE0028650}" uniqueName="17" name="Uitlaat3" queryTableFieldId="17" dataDxfId="22"/>
+    <tableColumn id="18" xr3:uid="{44A642CC-6F94-4E75-9796-1E854132BDCF}" uniqueName="18" name="Uitlaat4" queryTableFieldId="18" dataDxfId="21"/>
     <tableColumn id="19" xr3:uid="{57DE7CF8-A229-4842-A5AD-F43DA985FE87}" uniqueName="19" name="Column19" queryTableFieldId="24" dataDxfId="20">
-      <calculatedColumnFormula>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</calculatedColumnFormula>
+      <calculatedColumnFormula>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="20" xr3:uid="{21A9EECD-5880-4BC3-AE6A-60DE70363E02}" uniqueName="20" name="Column20" queryTableFieldId="25" dataDxfId="19">
-      <calculatedColumnFormula>IF(scraper__2[[#This Row],[Column5]]="",0,1)</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="21" xr3:uid="{E5E981D3-81F3-4AA1-86C9-66B3CA6C66ED}" uniqueName="21" name="Column21" queryTableFieldId="26" dataDxfId="18">
       <calculatedColumnFormula>scraper__2[[#This Row],[Column20]]*scraper__2[[#This Row],[Column19]]</calculatedColumnFormula>
@@ -2548,7 +2563,7 @@
   <dimension ref="A1:U88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2584,16 +2599,16 @@
         <v>278</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>288</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>289</v>
       </c>
       <c r="G1" t="s">
-        <v>64</v>
+        <v>290</v>
       </c>
       <c r="H1" t="s">
-        <v>65</v>
+        <v>291</v>
       </c>
       <c r="I1" t="s">
         <v>84</v>
@@ -2602,28 +2617,28 @@
         <v>85</v>
       </c>
       <c r="K1" t="s">
-        <v>68</v>
+        <v>169</v>
       </c>
       <c r="L1" t="s">
-        <v>69</v>
+        <v>170</v>
       </c>
       <c r="M1" t="s">
-        <v>70</v>
+        <v>171</v>
       </c>
       <c r="N1" t="s">
-        <v>71</v>
+        <v>172</v>
       </c>
       <c r="O1" t="s">
-        <v>72</v>
+        <v>287</v>
       </c>
       <c r="P1" t="s">
-        <v>73</v>
+        <v>264</v>
       </c>
       <c r="Q1" t="s">
-        <v>74</v>
+        <v>223</v>
       </c>
       <c r="R1" t="s">
-        <v>75</v>
+        <v>224</v>
       </c>
       <c r="S1" t="s">
         <v>281</v>
@@ -2675,11 +2690,11 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>5</v>
       </c>
       <c r="T2" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>1</v>
       </c>
       <c r="U2" s="2">
@@ -2720,11 +2735,11 @@
       </c>
       <c r="R3" s="2"/>
       <c r="S3" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>4</v>
       </c>
       <c r="T3" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U3" s="2">
@@ -2769,11 +2784,11 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>2</v>
       </c>
       <c r="T4" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U4" s="2">
@@ -2830,11 +2845,11 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>3</v>
       </c>
       <c r="T5" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>1</v>
       </c>
       <c r="U5" s="2">
@@ -2885,11 +2900,11 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>4</v>
       </c>
       <c r="T6" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>1</v>
       </c>
       <c r="U6" s="2">
@@ -2937,11 +2952,11 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>2</v>
       </c>
       <c r="T7" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U7" s="2">
@@ -2983,11 +2998,11 @@
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
       <c r="S8" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>4</v>
       </c>
       <c r="T8" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U8" s="2">
@@ -3029,11 +3044,11 @@
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
       <c r="S9" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>4</v>
       </c>
       <c r="T9" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U9" s="2">
@@ -3081,11 +3096,11 @@
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
       <c r="S10" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>5</v>
       </c>
       <c r="T10" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>1</v>
       </c>
       <c r="U10" s="2">
@@ -3130,11 +3145,11 @@
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>6</v>
       </c>
       <c r="T11" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>1</v>
       </c>
       <c r="U11" s="2">
@@ -3191,11 +3206,11 @@
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>10</v>
       </c>
       <c r="T12" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U12" s="2">
@@ -3254,11 +3269,11 @@
       </c>
       <c r="R13" s="2"/>
       <c r="S13" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>12</v>
       </c>
       <c r="T13" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>1</v>
       </c>
       <c r="U13" s="2">
@@ -3309,11 +3324,11 @@
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>2</v>
       </c>
       <c r="T14" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U14" s="2">
@@ -3358,11 +3373,11 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
       <c r="S15" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>4</v>
       </c>
       <c r="T15" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U15" s="2">
@@ -3419,11 +3434,11 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>1</v>
       </c>
       <c r="T16" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U16" s="2">
@@ -3480,11 +3495,11 @@
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
       <c r="S17" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>1</v>
       </c>
       <c r="T17" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U17" s="2">
@@ -3532,11 +3547,11 @@
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>4</v>
       </c>
       <c r="T18" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>1</v>
       </c>
       <c r="U18" s="2">
@@ -3584,11 +3599,11 @@
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
       <c r="S19" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>4</v>
       </c>
       <c r="T19" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>1</v>
       </c>
       <c r="U19" s="2">
@@ -3636,11 +3651,11 @@
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
       <c r="S20" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>4</v>
       </c>
       <c r="T20" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>1</v>
       </c>
       <c r="U20" s="2">
@@ -3697,11 +3712,11 @@
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
       <c r="S21" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>6</v>
       </c>
       <c r="T21" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>1</v>
       </c>
       <c r="U21" s="2">
@@ -3748,11 +3763,11 @@
       </c>
       <c r="R22" s="2"/>
       <c r="S22" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>1</v>
       </c>
       <c r="T22" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U22" s="2">
@@ -3793,11 +3808,11 @@
       </c>
       <c r="R23" s="2"/>
       <c r="S23" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>4</v>
       </c>
       <c r="T23" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U23" s="2">
@@ -3838,11 +3853,11 @@
       </c>
       <c r="R24" s="2"/>
       <c r="S24" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>5</v>
       </c>
       <c r="T24" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U24" s="2">
@@ -3885,11 +3900,11 @@
         <v>93</v>
       </c>
       <c r="S25" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>6</v>
       </c>
       <c r="T25" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U25" s="2">
@@ -3935,11 +3950,11 @@
         <v>93</v>
       </c>
       <c r="S26" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>8</v>
       </c>
       <c r="T26" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U26" s="2">
@@ -3986,11 +4001,11 @@
       </c>
       <c r="R27" s="2"/>
       <c r="S27" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>1</v>
       </c>
       <c r="T27" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U27" s="2">
@@ -4031,11 +4046,11 @@
       </c>
       <c r="R28" s="2"/>
       <c r="S28" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>3</v>
       </c>
       <c r="T28" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U28" s="2">
@@ -4076,11 +4091,11 @@
       </c>
       <c r="R29" s="2"/>
       <c r="S29" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>5</v>
       </c>
       <c r="T29" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U29" s="2">
@@ -4121,11 +4136,11 @@
       </c>
       <c r="R30" s="2"/>
       <c r="S30" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>5</v>
       </c>
       <c r="T30" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U30" s="2">
@@ -4169,11 +4184,11 @@
       </c>
       <c r="R31" s="2"/>
       <c r="S31" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>2</v>
       </c>
       <c r="T31" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U31" s="2">
@@ -4214,11 +4229,11 @@
       </c>
       <c r="R32" s="2"/>
       <c r="S32" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>2</v>
       </c>
       <c r="T32" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U32" s="2">
@@ -4258,11 +4273,11 @@
         <v>279</v>
       </c>
       <c r="S33" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>4</v>
       </c>
       <c r="T33" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U33" s="2">
@@ -4305,11 +4320,11 @@
         <v>279</v>
       </c>
       <c r="S34" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>5</v>
       </c>
       <c r="T34" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U34" s="2">
@@ -4357,11 +4372,11 @@
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
       <c r="S35" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>3</v>
       </c>
       <c r="T35" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>1</v>
       </c>
       <c r="U35" s="2">
@@ -4404,11 +4419,11 @@
         <v>279</v>
       </c>
       <c r="S36" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>6</v>
       </c>
       <c r="T36" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U36" s="2">
@@ -4451,11 +4466,11 @@
         <v>279</v>
       </c>
       <c r="S37" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>3</v>
       </c>
       <c r="T37" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U37" s="2">
@@ -4507,11 +4522,11 @@
         <v>279</v>
       </c>
       <c r="S38" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>2</v>
       </c>
       <c r="T38" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U38" s="2">
@@ -4568,11 +4583,11 @@
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
       <c r="S39" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>2</v>
       </c>
       <c r="T39" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>1</v>
       </c>
       <c r="U39" s="2">
@@ -4629,11 +4644,11 @@
       <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
       <c r="S40" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>2</v>
       </c>
       <c r="T40" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>1</v>
       </c>
       <c r="U40" s="2">
@@ -4679,11 +4694,11 @@
         <v>279</v>
       </c>
       <c r="S41" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>1</v>
       </c>
       <c r="T41" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U41" s="2">
@@ -4740,11 +4755,11 @@
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
       <c r="S42" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>2</v>
       </c>
       <c r="T42" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>1</v>
       </c>
       <c r="U42" s="2">
@@ -4789,11 +4804,11 @@
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
       <c r="S43" s="2">
-        <f>14-COUNTIF(scraper__2[[#This Row],[Column5]:[Column18]],"")</f>
+        <f>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</f>
         <v>6</v>
       </c>
       <c r="T43" s="2">
-        <f>IF(scraper__2[[#This Row],[Column5]]="",0,1)</f>
+        <f>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</f>
         <v>0</v>
       </c>
       <c r="U43" s="2">

</xml_diff>

<commit_message>
update excel with comments about simulations
</commit_message>
<xml_diff>
--- a/data/20181210_eag_info.xlsx
+++ b/data/20181210_eag_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\k\01projekt\17026004_WATERNET_Waterbalansen\05pyfiles\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2F8112-CA7D-4EE1-897B-D9444D5CDC02}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0166619-ED7D-48B6-9D5E-CAB072049ACE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="3" xr2:uid="{D42CEE2B-2D61-4AA0-9082-ECF2208A28A8}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1424" uniqueCount="313">
   <si>
     <t>ID</t>
   </si>
@@ -930,17 +930,71 @@
     <t>Opmerking</t>
   </si>
   <si>
-    <t>Water zakt te ver uit. Eerder simulatie niet (maar mogelijk zat QInMax toen nog niet goed)</t>
-  </si>
-  <si>
-    <t>Waterpeil niet juist, drain heel anders, veel dingen komen niet overeen…</t>
+    <t>2130-EAG-2</t>
+  </si>
+  <si>
+    <t>3110-EAG-1</t>
+  </si>
+  <si>
+    <t>q_cso iets anders dan in Excel. Poel en dijkslek inlaat zijn eerst ValueSeries en daarna handmatig ingevoerde reeks. ValueSeries ontbreekt nu uit reeksen.csv.</t>
+  </si>
+  <si>
+    <t>intrek heeft een minimum in Excel die niet in Python staat. Peil, inlaat en uitlaat waarshcijnlijk om die reden ook fout.</t>
+  </si>
+  <si>
+    <t>intrek en drain niet juist. q_cso ook iets anders maar ws minder groot probleem. Hopelijk alle verschillen functie van intrek fout</t>
+  </si>
+  <si>
+    <t>peil totaal anders, ontbrekende ValueSeries lijkt het bij verschil in drain en berekende uitlaat. Eerst peil beschouwen, dan verder kijken.</t>
+  </si>
+  <si>
+    <t>verschil intrek, daardoor verschil in inlaat, uitlaat en peil? Hoge piek in uitspoeling aan begin, waardoor?</t>
+  </si>
+  <si>
+    <t>Teveel inlaat, mogelijk iets met peil hTargets? Ook uitlaat klopt niet maar ws als gevolg van iets anders.</t>
+  </si>
+  <si>
+    <t>Goed</t>
+  </si>
+  <si>
+    <t>Verschil uitspoeling, Python heeft minimum grens, Excel niet. Verschil q_cso.</t>
+  </si>
+  <si>
+    <t>Verschil uitspoeling, missende ValueSeries lijkt het in verschil in uitlaat. Q_cso anders. Geen inlaat in Excel, wel in Python af en toe.</t>
+  </si>
+  <si>
+    <t>Later kwel en wegzijging reeksen in Excel niet in Python ingevoerd. Beginfase verschil door peil? In excel niet onder ondergrens, in python wel.</t>
+  </si>
+  <si>
+    <t>Goed (minimaal piekje bij begin intrek)</t>
+  </si>
+  <si>
+    <t>Iets fout met peil berekening</t>
+  </si>
+  <si>
+    <t>Verschil intrek, verschil uitspoeling, verschil peil.</t>
+  </si>
+  <si>
+    <t>Verschil uitspoeling (systematisch), verschil q_cso, klein verschil peil, veel te veel uitlaat (geen uitlaat in Excel)</t>
+  </si>
+  <si>
+    <t>Goed (verschil millimeters in peil, teveel inlaat en uitlaat, maar verschil mogelijk veroorzaakt door verdamping?)</t>
+  </si>
+  <si>
+    <t>Verschil uitspoeling (systematisch), verschil q_cso, peil ook niet goed.</t>
+  </si>
+  <si>
+    <t>Goed? (minimaal systematisch verschil uitspoeling, verschil uitlaat en inlaat door verdamping?)</t>
+  </si>
+  <si>
+    <t>intrek verschil, piek uitspoeling aan begin (kleine fout)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -956,8 +1010,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -970,6 +1031,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -980,50 +1046,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="42">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1141,6 +1180,36 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1215,31 +1284,31 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A2D62C0A-4B94-4D27-B2C8-F8018093AED4}" name="scraper__2" displayName="scraper__2" ref="A1:U43" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:U43" xr:uid="{E94C13C0-EE89-44BC-9695-1FBC7081F57E}"/>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{1DC9222B-85D5-43C6-AD17-EAB2845B0DF8}" uniqueName="1" name="EAG" queryTableFieldId="1" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{FEA2244A-36C6-4F74-B58F-FB49D89DD0CC}" uniqueName="2" name="Neerslag" queryTableFieldId="2" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{C49BF7A5-0F26-44EA-BC98-5CEF0772D30C}" uniqueName="3" name="Verdamping" queryTableFieldId="3" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{A7163F6B-1176-4B2E-8307-A9A79372D676}" uniqueName="4" name="Peil" queryTableFieldId="4" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{67EE6766-4720-4FC8-ADA1-AC30BCB9E382}" uniqueName="5" name="Gemaal1" queryTableFieldId="5" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{3452F98B-458D-422A-9EAC-3BA6259A959F}" uniqueName="6" name="Gemaal2" queryTableFieldId="6" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{E2BBD6F6-1AFB-4AF2-A6DB-C1B78A7D8E7E}" uniqueName="7" name="Gemaal3" queryTableFieldId="7" dataDxfId="35"/>
-    <tableColumn id="8" xr3:uid="{D8E8BA9C-B2E0-4A39-A11D-F29FCC5B8608}" uniqueName="8" name="Gemaal4" queryTableFieldId="8" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{72B32F7F-D21D-4B36-B0C0-2260DCB96323}" uniqueName="9" name="Inlaat voor calibratie" queryTableFieldId="9" dataDxfId="33"/>
-    <tableColumn id="10" xr3:uid="{D02B5E2F-FB46-441A-A699-CCF8EBCFDD16}" uniqueName="10" name="gemengd gerioleerd stelsel m3/d/ha" queryTableFieldId="10" dataDxfId="32"/>
-    <tableColumn id="11" xr3:uid="{F04540CE-2CAF-4EBF-B51E-4CC6BD370C76}" uniqueName="11" name="Inlaat1" queryTableFieldId="11" dataDxfId="31"/>
-    <tableColumn id="12" xr3:uid="{A2C87C34-3238-4479-AC31-07AE603A509A}" uniqueName="12" name="Inlaat2" queryTableFieldId="12" dataDxfId="30"/>
-    <tableColumn id="13" xr3:uid="{816668FE-6184-4D7F-B44B-D2FC05326D93}" uniqueName="13" name="Inlaat3" queryTableFieldId="13" dataDxfId="29"/>
-    <tableColumn id="14" xr3:uid="{EA0BC37D-0CEB-4296-82C3-501C31DBA056}" uniqueName="14" name="Inlaat4" queryTableFieldId="14" dataDxfId="28"/>
-    <tableColumn id="15" xr3:uid="{B3CE4A0B-0D02-4C8C-A562-227658C3108E}" uniqueName="15" name="Uitlaat1" queryTableFieldId="15" dataDxfId="27"/>
-    <tableColumn id="16" xr3:uid="{E1CB06E9-17AD-4E15-9093-F178C4020DCB}" uniqueName="16" name="Uitlaat2" queryTableFieldId="16" dataDxfId="26"/>
-    <tableColumn id="17" xr3:uid="{EABA0519-4E9E-4B4C-A8E0-09ECE0028650}" uniqueName="17" name="Uitlaat3" queryTableFieldId="17" dataDxfId="25"/>
-    <tableColumn id="18" xr3:uid="{44A642CC-6F94-4E75-9796-1E854132BDCF}" uniqueName="18" name="Uitlaat4" queryTableFieldId="18" dataDxfId="24"/>
-    <tableColumn id="19" xr3:uid="{57DE7CF8-A229-4842-A5AD-F43DA985FE87}" uniqueName="19" name="Column19" queryTableFieldId="24" dataDxfId="23">
+    <tableColumn id="1" xr3:uid="{1DC9222B-85D5-43C6-AD17-EAB2845B0DF8}" uniqueName="1" name="EAG" queryTableFieldId="1" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{FEA2244A-36C6-4F74-B58F-FB49D89DD0CC}" uniqueName="2" name="Neerslag" queryTableFieldId="2" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{C49BF7A5-0F26-44EA-BC98-5CEF0772D30C}" uniqueName="3" name="Verdamping" queryTableFieldId="3" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{A7163F6B-1176-4B2E-8307-A9A79372D676}" uniqueName="4" name="Peil" queryTableFieldId="4" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{67EE6766-4720-4FC8-ADA1-AC30BCB9E382}" uniqueName="5" name="Gemaal1" queryTableFieldId="5" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{3452F98B-458D-422A-9EAC-3BA6259A959F}" uniqueName="6" name="Gemaal2" queryTableFieldId="6" dataDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{E2BBD6F6-1AFB-4AF2-A6DB-C1B78A7D8E7E}" uniqueName="7" name="Gemaal3" queryTableFieldId="7" dataDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{D8E8BA9C-B2E0-4A39-A11D-F29FCC5B8608}" uniqueName="8" name="Gemaal4" queryTableFieldId="8" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{72B32F7F-D21D-4B36-B0C0-2260DCB96323}" uniqueName="9" name="Inlaat voor calibratie" queryTableFieldId="9" dataDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{D02B5E2F-FB46-441A-A699-CCF8EBCFDD16}" uniqueName="10" name="gemengd gerioleerd stelsel m3/d/ha" queryTableFieldId="10" dataDxfId="29"/>
+    <tableColumn id="11" xr3:uid="{F04540CE-2CAF-4EBF-B51E-4CC6BD370C76}" uniqueName="11" name="Inlaat1" queryTableFieldId="11" dataDxfId="28"/>
+    <tableColumn id="12" xr3:uid="{A2C87C34-3238-4479-AC31-07AE603A509A}" uniqueName="12" name="Inlaat2" queryTableFieldId="12" dataDxfId="27"/>
+    <tableColumn id="13" xr3:uid="{816668FE-6184-4D7F-B44B-D2FC05326D93}" uniqueName="13" name="Inlaat3" queryTableFieldId="13" dataDxfId="26"/>
+    <tableColumn id="14" xr3:uid="{EA0BC37D-0CEB-4296-82C3-501C31DBA056}" uniqueName="14" name="Inlaat4" queryTableFieldId="14" dataDxfId="25"/>
+    <tableColumn id="15" xr3:uid="{B3CE4A0B-0D02-4C8C-A562-227658C3108E}" uniqueName="15" name="Uitlaat1" queryTableFieldId="15" dataDxfId="24"/>
+    <tableColumn id="16" xr3:uid="{E1CB06E9-17AD-4E15-9093-F178C4020DCB}" uniqueName="16" name="Uitlaat2" queryTableFieldId="16" dataDxfId="23"/>
+    <tableColumn id="17" xr3:uid="{EABA0519-4E9E-4B4C-A8E0-09ECE0028650}" uniqueName="17" name="Uitlaat3" queryTableFieldId="17" dataDxfId="22"/>
+    <tableColumn id="18" xr3:uid="{44A642CC-6F94-4E75-9796-1E854132BDCF}" uniqueName="18" name="Uitlaat4" queryTableFieldId="18" dataDxfId="21"/>
+    <tableColumn id="19" xr3:uid="{57DE7CF8-A229-4842-A5AD-F43DA985FE87}" uniqueName="19" name="Column19" queryTableFieldId="24" dataDxfId="20">
       <calculatedColumnFormula>14-COUNTIF(scraper__2[[#This Row],[Gemaal1]:[Uitlaat4]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{21A9EECD-5880-4BC3-AE6A-60DE70363E02}" uniqueName="20" name="Column20" queryTableFieldId="25" dataDxfId="22">
+    <tableColumn id="20" xr3:uid="{21A9EECD-5880-4BC3-AE6A-60DE70363E02}" uniqueName="20" name="Column20" queryTableFieldId="25" dataDxfId="19">
       <calculatedColumnFormula>IF(scraper__2[[#This Row],[Gemaal1]]="",0,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{E5E981D3-81F3-4AA1-86C9-66B3CA6C66ED}" uniqueName="21" name="Column21" queryTableFieldId="26" dataDxfId="21">
+    <tableColumn id="21" xr3:uid="{E5E981D3-81F3-4AA1-86C9-66B3CA6C66ED}" uniqueName="21" name="Column21" queryTableFieldId="26" dataDxfId="18">
       <calculatedColumnFormula>scraper__2[[#This Row],[Column20]]*scraper__2[[#This Row],[Column19]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1251,24 +1320,24 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4139B22A-235F-4E82-A1D1-BFD0D166F878}" name="scraper" displayName="scraper" ref="A1:R43" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:R43" xr:uid="{13A51400-D748-46E8-9E88-99681A155BFD}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{CF8E3824-B133-459A-9C94-2EB591C520BB}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{5A0E499A-29A3-4BE3-918D-E4EE9F3EE0CC}" uniqueName="2" name="Neerslag" queryTableFieldId="2" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{7358E1E1-9BD0-42C3-957D-D99F57B1D8CA}" uniqueName="3" name="Verdamping" queryTableFieldId="3" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{3C58EFC8-2D72-49CD-B858-C400358A015F}" uniqueName="4" name="Peil" queryTableFieldId="4" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{C3A8AAC4-66BC-4C5E-B098-CB8B4C21F04E}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{C383F028-BADC-4655-896D-6EE018CC419D}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{825E8200-D8C3-41E6-8A48-59C24E2BF76E}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{7DD17B82-84DB-404C-85E4-C3BE0F2FC4ED}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{3D2D24DE-1584-4943-B040-29CC3ED44C76}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{CBE73725-6B7F-4214-A40A-C189B7AE94BA}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{7856A649-B3DE-488A-9846-9C3B7FAA5540}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{CA4FA753-73BC-4D0E-8E1A-35D5AA558FFA}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="9"/>
-    <tableColumn id="13" xr3:uid="{1645277E-6088-4067-A01A-2C45A89E0131}" uniqueName="13" name="Column13" queryTableFieldId="13" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{ED34940E-5D67-421C-A526-EA7E40F0DC7E}" uniqueName="14" name="Column14" queryTableFieldId="14" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{9E8F673D-9585-4837-A024-045CD1029E5C}" uniqueName="15" name="Column15" queryTableFieldId="15" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{B36AAEB5-635A-4619-883C-306DBC85068B}" uniqueName="16" name="Column16" queryTableFieldId="16" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{AB564CC6-5A1A-4F0F-B58D-7187EB59E0E7}" uniqueName="17" name="Column17" queryTableFieldId="17" dataDxfId="4"/>
-    <tableColumn id="18" xr3:uid="{AEB4B351-72B0-4413-95CD-D8C249F1F4EA}" uniqueName="18" name="Column18" queryTableFieldId="18" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{CF8E3824-B133-459A-9C94-2EB591C520BB}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{5A0E499A-29A3-4BE3-918D-E4EE9F3EE0CC}" uniqueName="2" name="Neerslag" queryTableFieldId="2" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{7358E1E1-9BD0-42C3-957D-D99F57B1D8CA}" uniqueName="3" name="Verdamping" queryTableFieldId="3" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{3C58EFC8-2D72-49CD-B858-C400358A015F}" uniqueName="4" name="Peil" queryTableFieldId="4" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{C3A8AAC4-66BC-4C5E-B098-CB8B4C21F04E}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{C383F028-BADC-4655-896D-6EE018CC419D}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{825E8200-D8C3-41E6-8A48-59C24E2BF76E}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{7DD17B82-84DB-404C-85E4-C3BE0F2FC4ED}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{3D2D24DE-1584-4943-B040-29CC3ED44C76}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{CBE73725-6B7F-4214-A40A-C189B7AE94BA}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{7856A649-B3DE-488A-9846-9C3B7FAA5540}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{CA4FA753-73BC-4D0E-8E1A-35D5AA558FFA}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{1645277E-6088-4067-A01A-2C45A89E0131}" uniqueName="13" name="Column13" queryTableFieldId="13" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{ED34940E-5D67-421C-A526-EA7E40F0DC7E}" uniqueName="14" name="Column14" queryTableFieldId="14" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{9E8F673D-9585-4837-A024-045CD1029E5C}" uniqueName="15" name="Column15" queryTableFieldId="15" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{B36AAEB5-635A-4619-883C-306DBC85068B}" uniqueName="16" name="Column16" queryTableFieldId="16" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{AB564CC6-5A1A-4F0F-B58D-7187EB59E0E7}" uniqueName="17" name="Column17" queryTableFieldId="17" dataDxfId="1"/>
+    <tableColumn id="18" xr3:uid="{AEB4B351-72B0-4413-95CD-D8C249F1F4EA}" uniqueName="18" name="Column18" queryTableFieldId="18" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7945,13 +8014,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A45:R86">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
       <formula>"-"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10421,16 +10490,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B89B73A9-5C46-4377-93A2-CD682A826B15}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.6640625" customWidth="1"/>
+    <col min="2" max="2" width="124.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
@@ -10443,138 +10512,226 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>293</v>
       </c>
       <c r="B2" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="B8" s="5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="B9" s="5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+      <c r="B10" s="5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>10</v>
+      <c r="B11" s="5" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
+        <v>294</v>
+      </c>
+      <c r="B14" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+      <c r="B16" s="5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+      <c r="B17" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+      <c r="B18" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+      <c r="B19" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+      <c r="B20" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+      <c r="B21" s="5" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+      <c r="B22" s="5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+      <c r="B23" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+      <c r="B24" s="5" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+      <c r="B25" s="5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+      <c r="B26" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+      <c r="B27" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+      <c r="B28" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29" s="5" t="s">
         <v>24</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>